<commit_message>
Changes to image generation
</commit_message>
<xml_diff>
--- a/blog_config.xlsx
+++ b/blog_config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ivanstruk/Documents/GitHub/good-news/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7BFDC23-89BE-2546-AB82-C4C893A6ADB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B15CEA51-FBE1-C541-B4B5-2662DD9C14FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="83220" yWindow="3340" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{AC684F59-F628-C54A-AD30-D4C8ABAC84A6}"/>
+    <workbookView xWindow="16020" yWindow="3340" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{AC684F59-F628-C54A-AD30-D4C8ABAC84A6}"/>
   </bookViews>
   <sheets>
     <sheet name="weekly_scheduler" sheetId="3" r:id="rId1"/>
@@ -817,10 +817,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1211,15 +1211,15 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
@@ -1801,79 +1801,79 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.1640625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="106.6640625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="21.1640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="106.6640625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="85" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="85" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="68" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="68" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="68" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="68" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="85" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="85" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>70</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Refactored Ask Ana translation management
</commit_message>
<xml_diff>
--- a/blog_config.xlsx
+++ b/blog_config.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ivanstruk/Documents/GitHub/good-news/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{500DCC4C-F8D2-D94B-8A12-23607112896A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{490C8B3E-AEA7-5743-8E42-69F8E18125A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="75360" yWindow="2920" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{AC684F59-F628-C54A-AD30-D4C8ABAC84A6}"/>
+    <workbookView xWindow="42400" yWindow="2660" windowWidth="28040" windowHeight="17440" activeTab="4" xr2:uid="{AC684F59-F628-C54A-AD30-D4C8ABAC84A6}"/>
   </bookViews>
   <sheets>
     <sheet name="weekly_scheduler" sheetId="3" r:id="rId1"/>
     <sheet name="sources" sheetId="1" r:id="rId2"/>
     <sheet name="image_prompts" sheetId="4" r:id="rId3"/>
     <sheet name="blocked_domains" sheetId="2" r:id="rId4"/>
+    <sheet name="lang_config" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">sources!$A$1:$G$1</definedName>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="90">
   <si>
     <t>RSS</t>
   </si>
@@ -274,6 +275,54 @@
   </si>
   <si>
     <t>Latest News</t>
+  </si>
+  <si>
+    <t>lang</t>
+  </si>
+  <si>
+    <t>post</t>
+  </si>
+  <si>
+    <t>run</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>German</t>
+  </si>
+  <si>
+    <t>Russian</t>
+  </si>
+  <si>
+    <t>Chinese (simplified)</t>
+  </si>
+  <si>
+    <t>Hindi</t>
+  </si>
+  <si>
+    <t>Spanish</t>
+  </si>
+  <si>
+    <t>French</t>
+  </si>
+  <si>
+    <t>de</t>
+  </si>
+  <si>
+    <t>ru</t>
+  </si>
+  <si>
+    <t>zh</t>
+  </si>
+  <si>
+    <t>hi</t>
+  </si>
+  <si>
+    <t>es</t>
+  </si>
+  <si>
+    <t>fr</t>
   </si>
 </sst>
 </file>
@@ -1376,7 +1425,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19E55AEB-D2F4-EE41-86F8-038347F2C987}">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
@@ -2043,4 +2092,117 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01EB545A-A6FB-6D44-9886-FE4E01916CDF}">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" t="b">
+        <v>1</v>
+      </c>
+      <c r="C4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" t="b">
+        <v>0</v>
+      </c>
+      <c r="C5" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B7" t="b">
+        <v>1</v>
+      </c>
+      <c r="C7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>